<commit_message>
add post sample for dataElement/ optionSet/ options
</commit_message>
<xml_diff>
--- a/sample-format/dataValueSet.xlsx
+++ b/sample-format/dataValueSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B306DB09-B5B8-4167-817D-63CED2C419AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F4ECD8-F5D7-4D84-8B04-62725C6C7B29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>dataElementUID</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>dataValue</t>
+  </si>
+  <si>
+    <t>pGeBz8X2jRq</t>
+  </si>
+  <si>
+    <t>yHSAPCLxecr</t>
+  </si>
+  <si>
+    <t>WTSe3FmRFmD</t>
   </si>
 </sst>
 </file>
@@ -897,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E53635"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -929,6 +938,23 @@
       </c>
       <c r="F1" s="2"/>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1">
+        <v>202007</v>
+      </c>
+      <c r="E2" s="1">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update format of datavalue set import
</commit_message>
<xml_diff>
--- a/sample-format/dataValueSet.xlsx
+++ b/sample-format/dataValueSet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F4ECD8-F5D7-4D84-8B04-62725C6C7B29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A70A11D-0A72-479A-92E8-9B108CB0F53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataValueSet" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>dataElementUID</t>
   </si>
@@ -47,13 +47,13 @@
     <t>dataValue</t>
   </si>
   <si>
-    <t>pGeBz8X2jRq</t>
+    <t>HllvX50cXC0</t>
   </si>
   <si>
-    <t>yHSAPCLxecr</t>
+    <t>Cx3VCA0dbrk</t>
   </si>
   <si>
-    <t>WTSe3FmRFmD</t>
+    <t>Ml4vtfj16Zw</t>
   </si>
 </sst>
 </file>
@@ -543,13 +543,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -906,28 +912,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:E331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.453125" style="1" customWidth="1"/>
     <col min="4" max="5" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -936,24 +943,2581 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1">
-        <v>202007</v>
+      <c r="D2" s="4">
+        <v>20220405</v>
       </c>
       <c r="E2" s="1">
-        <v>8</v>
+        <v>80</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4">
+        <v>20220406</v>
+      </c>
+      <c r="E3" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B4" s="2"/>
+      <c r="C4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="C5"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="2"/>
+      <c r="C6"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="2"/>
+      <c r="C7"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="2"/>
+      <c r="C8"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="2"/>
+      <c r="C9"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="2"/>
+      <c r="C10"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="2"/>
+      <c r="C11"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B12" s="2"/>
+      <c r="C12"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="2"/>
+      <c r="C14"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="2"/>
+      <c r="C15"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="2"/>
+      <c r="C16"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="2"/>
+      <c r="C17"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+      <c r="C18"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="2"/>
+      <c r="C19"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="2"/>
+      <c r="C20"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B21" s="2"/>
+      <c r="C21"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B23" s="2"/>
+      <c r="C23"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B24" s="2"/>
+      <c r="C24"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B25" s="2"/>
+      <c r="C25"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B26" s="2"/>
+      <c r="C26"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B27" s="2"/>
+      <c r="C27"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B28" s="2"/>
+      <c r="C28"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B29" s="2"/>
+      <c r="C29"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B30" s="2"/>
+      <c r="C30"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B31" s="2"/>
+      <c r="C31"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B32" s="2"/>
+      <c r="C32"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B33" s="2"/>
+      <c r="C33"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="2"/>
+      <c r="C34"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="2"/>
+      <c r="C35"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B36" s="2"/>
+      <c r="C36"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B37" s="2"/>
+      <c r="C37"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B38" s="2"/>
+      <c r="C38"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B39" s="2"/>
+      <c r="C39"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40" s="2"/>
+      <c r="C40"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B41" s="2"/>
+      <c r="C41"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B42" s="2"/>
+      <c r="C42"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B43" s="2"/>
+      <c r="C43"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B44" s="2"/>
+      <c r="C44"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B45" s="2"/>
+      <c r="C45"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B46" s="2"/>
+      <c r="C46"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B47" s="2"/>
+      <c r="C47"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B48" s="2"/>
+      <c r="C48"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B49" s="2"/>
+      <c r="C49"/>
+      <c r="D49" s="4"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B50" s="2"/>
+      <c r="C50"/>
+      <c r="D50" s="4"/>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B51" s="2"/>
+      <c r="C51"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B52" s="2"/>
+      <c r="C52"/>
+      <c r="D52" s="4"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B53" s="2"/>
+      <c r="C53"/>
+      <c r="D53" s="4"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B54" s="2"/>
+      <c r="C54"/>
+      <c r="D54" s="4"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B55" s="2"/>
+      <c r="C55"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B56" s="2"/>
+      <c r="C56"/>
+      <c r="D56" s="4"/>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B57" s="2"/>
+      <c r="C57"/>
+      <c r="D57" s="4"/>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B58" s="2"/>
+      <c r="C58"/>
+      <c r="D58" s="4"/>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B59" s="2"/>
+      <c r="C59"/>
+      <c r="D59" s="4"/>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B60" s="2"/>
+      <c r="C60"/>
+      <c r="D60" s="4"/>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B61" s="2"/>
+      <c r="C61"/>
+      <c r="D61" s="4"/>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B62" s="2"/>
+      <c r="C62"/>
+      <c r="D62" s="4"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B63" s="2"/>
+      <c r="C63"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B64" s="2"/>
+      <c r="C64"/>
+      <c r="D64" s="4"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B65" s="2"/>
+      <c r="C65"/>
+      <c r="D65" s="4"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B66" s="2"/>
+      <c r="C66"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B67" s="2"/>
+      <c r="C67"/>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B68" s="2"/>
+      <c r="C68"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B69" s="2"/>
+      <c r="C69"/>
+      <c r="D69" s="4"/>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B70" s="2"/>
+      <c r="C70"/>
+      <c r="D70" s="4"/>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B71" s="2"/>
+      <c r="C71"/>
+      <c r="D71" s="4"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B72" s="2"/>
+      <c r="C72"/>
+      <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B73" s="2"/>
+      <c r="C73"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B74" s="2"/>
+      <c r="C74"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B75" s="2"/>
+      <c r="C75"/>
+      <c r="D75" s="4"/>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B76" s="2"/>
+      <c r="C76"/>
+      <c r="D76" s="4"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B77" s="2"/>
+      <c r="C77"/>
+      <c r="D77" s="4"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B78" s="2"/>
+      <c r="C78"/>
+      <c r="D78" s="4"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B79" s="2"/>
+      <c r="C79"/>
+      <c r="D79" s="4"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B80" s="2"/>
+      <c r="C80"/>
+      <c r="D80" s="4"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B81" s="2"/>
+      <c r="C81"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B82" s="2"/>
+      <c r="C82"/>
+      <c r="D82" s="4"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B83" s="2"/>
+      <c r="C83"/>
+      <c r="D83" s="4"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B84" s="2"/>
+      <c r="C84"/>
+      <c r="D84" s="4"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B85" s="2"/>
+      <c r="C85"/>
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B86" s="2"/>
+      <c r="C86"/>
+      <c r="D86" s="4"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B87" s="2"/>
+      <c r="C87"/>
+      <c r="D87" s="4"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B88" s="2"/>
+      <c r="C88"/>
+      <c r="D88" s="4"/>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B89" s="2"/>
+      <c r="C89"/>
+      <c r="D89" s="4"/>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B90" s="2"/>
+      <c r="C90"/>
+      <c r="D90" s="4"/>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B91" s="2"/>
+      <c r="C91"/>
+      <c r="D91" s="4"/>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B92" s="2"/>
+      <c r="C92"/>
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B93" s="2"/>
+      <c r="C93"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B94" s="2"/>
+      <c r="C94"/>
+      <c r="D94" s="4"/>
+    </row>
+    <row r="95" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B95" s="2"/>
+      <c r="C95"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B96" s="2"/>
+      <c r="C96"/>
+      <c r="D96" s="4"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B97" s="2"/>
+      <c r="C97"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B98" s="2"/>
+      <c r="C98"/>
+      <c r="D98" s="4"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B99" s="2"/>
+      <c r="C99"/>
+      <c r="D99" s="4"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B100" s="2"/>
+      <c r="C100"/>
+      <c r="D100" s="4"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B101" s="2"/>
+      <c r="C101"/>
+      <c r="D101" s="4"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B102" s="2"/>
+      <c r="C102"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B103" s="2"/>
+      <c r="C103"/>
+      <c r="D103" s="4"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B104" s="2"/>
+      <c r="C104"/>
+      <c r="D104" s="4"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B105" s="2"/>
+      <c r="C105"/>
+      <c r="D105" s="4"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B106" s="2"/>
+      <c r="C106"/>
+      <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B107" s="2"/>
+      <c r="C107"/>
+      <c r="D107" s="4"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B108" s="2"/>
+      <c r="C108"/>
+      <c r="D108" s="4"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B109" s="2"/>
+      <c r="C109"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B110" s="2"/>
+      <c r="C110"/>
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B111" s="2"/>
+      <c r="C111"/>
+      <c r="D111" s="4"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B112" s="2"/>
+      <c r="C112"/>
+      <c r="D112" s="4"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B113" s="2"/>
+      <c r="C113"/>
+      <c r="D113" s="4"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B114" s="2"/>
+      <c r="C114"/>
+      <c r="D114" s="4"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B115" s="2"/>
+      <c r="C115"/>
+      <c r="D115" s="4"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B116" s="2"/>
+      <c r="C116"/>
+      <c r="D116" s="4"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B117" s="2"/>
+      <c r="C117"/>
+      <c r="D117" s="4"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B118" s="2"/>
+      <c r="C118"/>
+      <c r="D118" s="4"/>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B119" s="2"/>
+      <c r="C119"/>
+      <c r="D119" s="4"/>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B120" s="2"/>
+      <c r="C120"/>
+      <c r="D120" s="4"/>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B121" s="2"/>
+      <c r="C121"/>
+      <c r="D121" s="4"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B122" s="2"/>
+      <c r="C122"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B123" s="2"/>
+      <c r="C123"/>
+      <c r="D123" s="4"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B124" s="2"/>
+      <c r="C124"/>
+      <c r="D124" s="4"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B125" s="2"/>
+      <c r="C125"/>
+      <c r="D125" s="4"/>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B126" s="2"/>
+      <c r="C126"/>
+      <c r="D126" s="4"/>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B127" s="2"/>
+      <c r="C127"/>
+      <c r="D127" s="4"/>
+    </row>
+    <row r="128" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B128" s="2"/>
+      <c r="C128"/>
+      <c r="D128" s="4"/>
+    </row>
+    <row r="129" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B129" s="2"/>
+      <c r="C129"/>
+      <c r="D129" s="4"/>
+    </row>
+    <row r="130" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B130" s="2"/>
+      <c r="C130"/>
+      <c r="D130" s="4"/>
+    </row>
+    <row r="131" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B131" s="2"/>
+      <c r="C131"/>
+      <c r="D131" s="4"/>
+    </row>
+    <row r="132" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B132" s="2"/>
+      <c r="C132"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B133" s="2"/>
+      <c r="C133"/>
+      <c r="D133" s="4"/>
+    </row>
+    <row r="134" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B134" s="2"/>
+      <c r="C134"/>
+      <c r="D134" s="4"/>
+    </row>
+    <row r="135" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B135" s="2"/>
+      <c r="C135"/>
+      <c r="D135" s="4"/>
+    </row>
+    <row r="136" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B136" s="2"/>
+      <c r="C136"/>
+      <c r="D136" s="4"/>
+    </row>
+    <row r="137" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B137" s="2"/>
+      <c r="C137"/>
+      <c r="D137" s="4"/>
+    </row>
+    <row r="138" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B138" s="2"/>
+      <c r="C138"/>
+      <c r="D138" s="4"/>
+    </row>
+    <row r="139" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B139" s="2"/>
+      <c r="C139"/>
+      <c r="D139" s="4"/>
+    </row>
+    <row r="140" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B140" s="2"/>
+      <c r="C140"/>
+      <c r="D140" s="4"/>
+    </row>
+    <row r="141" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B141" s="2"/>
+      <c r="C141"/>
+      <c r="D141" s="4"/>
+    </row>
+    <row r="142" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B142" s="2"/>
+      <c r="C142"/>
+      <c r="D142" s="4"/>
+    </row>
+    <row r="143" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B143" s="2"/>
+      <c r="C143"/>
+      <c r="D143" s="4"/>
+    </row>
+    <row r="144" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B144" s="2"/>
+      <c r="C144"/>
+      <c r="D144" s="4"/>
+    </row>
+    <row r="145" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B145" s="2"/>
+      <c r="C145"/>
+      <c r="D145" s="4"/>
+    </row>
+    <row r="146" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B146" s="2"/>
+      <c r="C146"/>
+      <c r="D146" s="4"/>
+    </row>
+    <row r="147" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B147" s="2"/>
+      <c r="C147"/>
+      <c r="D147" s="4"/>
+    </row>
+    <row r="148" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B148" s="2"/>
+      <c r="C148"/>
+      <c r="D148" s="4"/>
+    </row>
+    <row r="149" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B149" s="2"/>
+      <c r="C149"/>
+      <c r="D149" s="4"/>
+    </row>
+    <row r="150" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B150" s="2"/>
+      <c r="C150"/>
+      <c r="D150" s="4"/>
+    </row>
+    <row r="151" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B151" s="2"/>
+      <c r="C151"/>
+      <c r="D151" s="4"/>
+    </row>
+    <row r="152" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B152" s="2"/>
+      <c r="C152"/>
+      <c r="D152" s="4"/>
+    </row>
+    <row r="153" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B153" s="2"/>
+      <c r="C153"/>
+      <c r="D153" s="4"/>
+    </row>
+    <row r="154" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B154" s="2"/>
+      <c r="C154"/>
+      <c r="D154" s="4"/>
+    </row>
+    <row r="155" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B155" s="2"/>
+      <c r="C155"/>
+      <c r="D155" s="4"/>
+    </row>
+    <row r="156" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B156" s="2"/>
+      <c r="C156"/>
+      <c r="D156" s="4"/>
+    </row>
+    <row r="157" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B157" s="2"/>
+      <c r="C157"/>
+      <c r="D157" s="4"/>
+    </row>
+    <row r="158" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B158" s="2"/>
+      <c r="C158"/>
+      <c r="D158" s="4"/>
+    </row>
+    <row r="159" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B159" s="2"/>
+      <c r="C159"/>
+      <c r="D159" s="4"/>
+    </row>
+    <row r="160" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B160" s="2"/>
+      <c r="C160"/>
+      <c r="D160" s="4"/>
+    </row>
+    <row r="161" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B161" s="2"/>
+      <c r="C161"/>
+      <c r="D161" s="4"/>
+    </row>
+    <row r="162" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B162" s="2"/>
+      <c r="C162"/>
+      <c r="D162" s="4"/>
+    </row>
+    <row r="163" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B163" s="2"/>
+      <c r="C163"/>
+      <c r="D163" s="4"/>
+    </row>
+    <row r="164" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B164" s="2"/>
+      <c r="C164"/>
+      <c r="D164" s="4"/>
+    </row>
+    <row r="165" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B165" s="2"/>
+      <c r="C165"/>
+      <c r="D165" s="4"/>
+    </row>
+    <row r="166" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B166" s="2"/>
+      <c r="C166"/>
+      <c r="D166" s="4"/>
+    </row>
+    <row r="167" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B167" s="2"/>
+      <c r="C167"/>
+      <c r="D167" s="4"/>
+    </row>
+    <row r="168" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B168" s="2"/>
+      <c r="C168"/>
+      <c r="D168" s="4"/>
+    </row>
+    <row r="169" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B169" s="2"/>
+      <c r="C169"/>
+      <c r="D169" s="4"/>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B170" s="2"/>
+      <c r="C170"/>
+      <c r="D170" s="4"/>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B171" s="2"/>
+      <c r="C171"/>
+      <c r="D171" s="4"/>
+    </row>
+    <row r="172" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B172" s="2"/>
+      <c r="C172"/>
+      <c r="D172" s="4"/>
+    </row>
+    <row r="173" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B173" s="2"/>
+      <c r="C173"/>
+      <c r="D173" s="4"/>
+    </row>
+    <row r="174" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B174" s="2"/>
+      <c r="C174"/>
+      <c r="D174" s="4"/>
+    </row>
+    <row r="175" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B175" s="2"/>
+      <c r="C175"/>
+      <c r="D175" s="4"/>
+    </row>
+    <row r="176" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B176" s="2"/>
+      <c r="C176"/>
+      <c r="D176" s="4"/>
+    </row>
+    <row r="177" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B177" s="2"/>
+      <c r="C177"/>
+      <c r="D177" s="4"/>
+    </row>
+    <row r="178" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B178" s="2"/>
+      <c r="C178"/>
+      <c r="D178" s="4"/>
+    </row>
+    <row r="179" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B179" s="2"/>
+      <c r="C179"/>
+      <c r="D179" s="4"/>
+    </row>
+    <row r="180" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B180" s="2"/>
+      <c r="C180"/>
+      <c r="D180" s="4"/>
+    </row>
+    <row r="181" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B181" s="2"/>
+      <c r="C181"/>
+      <c r="D181" s="4"/>
+    </row>
+    <row r="182" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B182" s="2"/>
+      <c r="C182"/>
+      <c r="D182" s="4"/>
+    </row>
+    <row r="183" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B183" s="2"/>
+      <c r="C183"/>
+      <c r="D183" s="4"/>
+    </row>
+    <row r="184" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B184" s="2"/>
+      <c r="C184"/>
+      <c r="D184" s="4"/>
+    </row>
+    <row r="185" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B185" s="2"/>
+      <c r="C185"/>
+      <c r="D185" s="4"/>
+    </row>
+    <row r="186" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B186" s="2"/>
+      <c r="C186"/>
+      <c r="D186" s="4"/>
+    </row>
+    <row r="187" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B187" s="2"/>
+      <c r="C187"/>
+      <c r="D187" s="4"/>
+    </row>
+    <row r="188" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B188" s="2"/>
+      <c r="C188"/>
+      <c r="D188" s="4"/>
+    </row>
+    <row r="189" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B189" s="2"/>
+      <c r="C189"/>
+      <c r="D189" s="4"/>
+    </row>
+    <row r="190" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B190" s="2"/>
+      <c r="C190"/>
+      <c r="D190" s="4"/>
+    </row>
+    <row r="191" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B191" s="2"/>
+      <c r="C191"/>
+      <c r="D191" s="4"/>
+    </row>
+    <row r="192" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B192" s="2"/>
+      <c r="C192"/>
+      <c r="D192" s="4"/>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B193" s="2"/>
+      <c r="C193"/>
+      <c r="D193" s="4"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B194" s="2"/>
+      <c r="C194"/>
+      <c r="D194" s="4"/>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B195" s="2"/>
+      <c r="C195"/>
+      <c r="D195" s="4"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B196" s="2"/>
+      <c r="C196"/>
+      <c r="D196" s="4"/>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B197" s="2"/>
+      <c r="C197"/>
+      <c r="D197" s="4"/>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B198" s="2"/>
+      <c r="C198"/>
+      <c r="D198" s="4"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B199" s="2"/>
+      <c r="C199"/>
+      <c r="D199" s="4"/>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B200" s="2"/>
+      <c r="C200"/>
+      <c r="D200" s="4"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B201" s="2"/>
+      <c r="C201"/>
+      <c r="D201" s="4"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B202" s="2"/>
+      <c r="C202"/>
+      <c r="D202" s="4"/>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B203" s="2"/>
+      <c r="C203"/>
+      <c r="D203" s="4"/>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B204" s="2"/>
+      <c r="C204"/>
+      <c r="D204" s="4"/>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B205" s="2"/>
+      <c r="C205"/>
+      <c r="D205" s="4"/>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B206" s="2"/>
+      <c r="C206"/>
+      <c r="D206" s="4"/>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B207" s="2"/>
+      <c r="C207"/>
+      <c r="D207" s="4"/>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B208" s="2"/>
+      <c r="C208"/>
+      <c r="D208" s="4"/>
+    </row>
+    <row r="209" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B209" s="2"/>
+      <c r="C209"/>
+      <c r="D209" s="4"/>
+    </row>
+    <row r="210" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B210" s="2"/>
+      <c r="C210"/>
+      <c r="D210" s="4"/>
+    </row>
+    <row r="211" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B211" s="2"/>
+      <c r="C211"/>
+      <c r="D211" s="4"/>
+    </row>
+    <row r="212" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B212" s="2"/>
+      <c r="C212"/>
+      <c r="D212" s="4"/>
+    </row>
+    <row r="213" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B213" s="2"/>
+      <c r="C213"/>
+      <c r="D213" s="4"/>
+    </row>
+    <row r="214" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B214" s="2"/>
+      <c r="C214"/>
+      <c r="D214" s="4"/>
+    </row>
+    <row r="215" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B215" s="2"/>
+      <c r="C215"/>
+      <c r="D215" s="4"/>
+    </row>
+    <row r="216" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B216" s="2"/>
+      <c r="C216"/>
+      <c r="D216" s="4"/>
+    </row>
+    <row r="217" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B217" s="2"/>
+      <c r="C217"/>
+      <c r="D217" s="4"/>
+    </row>
+    <row r="218" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B218" s="2"/>
+      <c r="C218"/>
+      <c r="D218" s="4"/>
+    </row>
+    <row r="219" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B219" s="2"/>
+      <c r="C219"/>
+      <c r="D219" s="4"/>
+    </row>
+    <row r="220" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B220" s="2"/>
+      <c r="C220"/>
+      <c r="D220" s="4"/>
+    </row>
+    <row r="221" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B221" s="2"/>
+      <c r="C221"/>
+      <c r="D221" s="4"/>
+    </row>
+    <row r="222" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B222" s="2"/>
+      <c r="C222"/>
+      <c r="D222" s="4"/>
+    </row>
+    <row r="223" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B223" s="2"/>
+      <c r="C223"/>
+      <c r="D223" s="4"/>
+    </row>
+    <row r="224" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B224" s="2"/>
+      <c r="C224"/>
+      <c r="D224" s="4"/>
+    </row>
+    <row r="225" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B225" s="2"/>
+      <c r="C225"/>
+      <c r="D225" s="4"/>
+    </row>
+    <row r="226" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B226" s="2"/>
+      <c r="C226"/>
+      <c r="D226" s="4"/>
+    </row>
+    <row r="227" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B227" s="2"/>
+      <c r="C227"/>
+      <c r="D227" s="4"/>
+    </row>
+    <row r="228" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B228" s="2"/>
+      <c r="C228"/>
+      <c r="D228" s="4"/>
+    </row>
+    <row r="229" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B229" s="2"/>
+      <c r="C229"/>
+      <c r="D229" s="4"/>
+    </row>
+    <row r="230" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B230" s="2"/>
+      <c r="C230"/>
+      <c r="D230" s="4"/>
+    </row>
+    <row r="231" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B231" s="2"/>
+      <c r="C231"/>
+      <c r="D231" s="4"/>
+    </row>
+    <row r="232" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B232" s="2"/>
+      <c r="C232"/>
+      <c r="D232" s="4"/>
+    </row>
+    <row r="233" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B233" s="2"/>
+      <c r="C233"/>
+      <c r="D233" s="4"/>
+    </row>
+    <row r="234" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B234" s="2"/>
+      <c r="C234"/>
+      <c r="D234" s="4"/>
+    </row>
+    <row r="235" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B235" s="2"/>
+      <c r="C235"/>
+      <c r="D235" s="4"/>
+    </row>
+    <row r="236" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B236" s="2"/>
+      <c r="C236"/>
+      <c r="D236" s="4"/>
+    </row>
+    <row r="237" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B237" s="2"/>
+      <c r="C237"/>
+      <c r="D237" s="4"/>
+    </row>
+    <row r="238" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B238" s="2"/>
+      <c r="C238"/>
+      <c r="D238" s="4"/>
+    </row>
+    <row r="239" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B239" s="2"/>
+      <c r="C239"/>
+      <c r="D239" s="4"/>
+    </row>
+    <row r="240" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B240" s="2"/>
+      <c r="C240"/>
+      <c r="D240" s="4"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B241" s="2"/>
+      <c r="C241"/>
+      <c r="D241" s="4"/>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B242" s="2"/>
+      <c r="C242"/>
+      <c r="D242" s="4"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B243" s="2"/>
+      <c r="C243"/>
+      <c r="D243" s="4"/>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B244" s="2"/>
+      <c r="C244"/>
+      <c r="D244" s="4"/>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B245" s="2"/>
+      <c r="C245"/>
+      <c r="D245" s="4"/>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B246" s="2"/>
+      <c r="C246"/>
+      <c r="D246" s="4"/>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B247" s="2"/>
+      <c r="C247"/>
+      <c r="D247" s="4"/>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B248" s="2"/>
+      <c r="C248"/>
+      <c r="D248" s="4"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B249" s="2"/>
+      <c r="C249"/>
+      <c r="D249" s="4"/>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B250" s="2"/>
+      <c r="C250"/>
+      <c r="D250" s="4"/>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B251" s="2"/>
+      <c r="C251"/>
+      <c r="D251" s="4"/>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B252" s="2"/>
+      <c r="C252"/>
+      <c r="D252" s="4"/>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B253" s="2"/>
+      <c r="C253"/>
+      <c r="D253" s="4"/>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B254" s="2"/>
+      <c r="C254"/>
+      <c r="D254" s="4"/>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B255" s="2"/>
+      <c r="C255"/>
+      <c r="D255" s="4"/>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B256" s="2"/>
+      <c r="C256"/>
+      <c r="D256" s="4"/>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B257" s="2"/>
+      <c r="C257"/>
+      <c r="D257" s="4"/>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B258" s="2"/>
+      <c r="C258"/>
+      <c r="D258" s="4"/>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B259" s="2"/>
+      <c r="C259"/>
+      <c r="D259" s="4"/>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B260" s="2"/>
+      <c r="C260"/>
+      <c r="D260" s="4"/>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B261" s="2"/>
+      <c r="C261"/>
+      <c r="D261" s="4"/>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B262" s="2"/>
+      <c r="C262"/>
+      <c r="D262" s="4"/>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B263" s="2"/>
+      <c r="C263"/>
+      <c r="D263" s="4"/>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B264" s="2"/>
+      <c r="C264"/>
+      <c r="D264" s="4"/>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B265" s="2"/>
+      <c r="C265"/>
+      <c r="D265" s="4"/>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B266" s="2"/>
+      <c r="C266"/>
+      <c r="D266" s="4"/>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B267" s="2"/>
+      <c r="C267"/>
+      <c r="D267" s="4"/>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B268" s="2"/>
+      <c r="C268"/>
+      <c r="D268" s="4"/>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B269" s="2"/>
+      <c r="C269"/>
+      <c r="D269" s="4"/>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B270" s="2"/>
+      <c r="C270"/>
+      <c r="D270" s="4"/>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B271" s="2"/>
+      <c r="C271"/>
+      <c r="D271" s="4"/>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B272" s="2"/>
+      <c r="C272"/>
+      <c r="D272" s="4"/>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B273" s="2"/>
+      <c r="C273"/>
+      <c r="D273" s="4"/>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B274" s="2"/>
+      <c r="C274"/>
+      <c r="D274" s="4"/>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B275" s="2"/>
+      <c r="C275"/>
+      <c r="D275" s="4"/>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B276" s="2"/>
+      <c r="C276"/>
+      <c r="D276" s="4"/>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B277" s="2"/>
+      <c r="C277"/>
+      <c r="D277" s="4"/>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B278" s="2"/>
+      <c r="C278"/>
+      <c r="D278" s="4"/>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B279" s="2"/>
+      <c r="C279"/>
+      <c r="D279" s="4"/>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B280" s="2"/>
+      <c r="C280"/>
+      <c r="D280" s="4"/>
+    </row>
+    <row r="281" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B281" s="2"/>
+      <c r="C281"/>
+      <c r="D281" s="4"/>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B282" s="2"/>
+      <c r="C282"/>
+      <c r="D282" s="4"/>
+    </row>
+    <row r="283" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B283" s="2"/>
+      <c r="C283"/>
+      <c r="D283" s="4"/>
+    </row>
+    <row r="284" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B284" s="2"/>
+      <c r="C284"/>
+      <c r="D284" s="4"/>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B285" s="2"/>
+      <c r="C285"/>
+      <c r="D285" s="4"/>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B286" s="2"/>
+      <c r="C286"/>
+      <c r="D286" s="4"/>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B287" s="2"/>
+      <c r="C287"/>
+      <c r="D287" s="4"/>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B288" s="2"/>
+      <c r="C288"/>
+      <c r="D288" s="4"/>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B289" s="2"/>
+      <c r="C289"/>
+      <c r="D289" s="4"/>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B290" s="2"/>
+      <c r="C290"/>
+      <c r="D290" s="4"/>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B291" s="2"/>
+      <c r="C291"/>
+      <c r="D291" s="4"/>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B292" s="2"/>
+      <c r="C292"/>
+      <c r="D292" s="4"/>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B293" s="2"/>
+      <c r="C293"/>
+      <c r="D293" s="4"/>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B294" s="2"/>
+      <c r="C294"/>
+      <c r="D294" s="4"/>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B295" s="2"/>
+      <c r="C295"/>
+      <c r="D295" s="4"/>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B296" s="2"/>
+      <c r="C296"/>
+      <c r="D296" s="4"/>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B297" s="2"/>
+      <c r="C297"/>
+      <c r="D297" s="4"/>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B298" s="2"/>
+      <c r="C298"/>
+      <c r="D298" s="4"/>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B299" s="2"/>
+      <c r="C299"/>
+      <c r="D299" s="4"/>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B300" s="2"/>
+      <c r="C300"/>
+      <c r="D300" s="4"/>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B301" s="2"/>
+      <c r="C301"/>
+      <c r="D301" s="4"/>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B302" s="2"/>
+      <c r="C302"/>
+      <c r="D302" s="4"/>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B303" s="2"/>
+      <c r="C303"/>
+      <c r="D303" s="4"/>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B304" s="2"/>
+      <c r="C304"/>
+      <c r="D304" s="4"/>
+    </row>
+    <row r="305" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B305" s="2"/>
+      <c r="C305"/>
+      <c r="D305" s="4"/>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B306" s="2"/>
+      <c r="C306"/>
+      <c r="D306" s="4"/>
+    </row>
+    <row r="307" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B307" s="2"/>
+      <c r="C307"/>
+      <c r="D307" s="4"/>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B308" s="2"/>
+      <c r="C308"/>
+      <c r="D308" s="4"/>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B309" s="2"/>
+      <c r="C309"/>
+      <c r="D309" s="4"/>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B310" s="2"/>
+      <c r="C310"/>
+      <c r="D310" s="4"/>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B311" s="2"/>
+      <c r="C311"/>
+      <c r="D311" s="4"/>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B312" s="2"/>
+      <c r="C312"/>
+      <c r="D312" s="4"/>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B313" s="2"/>
+      <c r="C313"/>
+      <c r="D313" s="4"/>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B314" s="2"/>
+      <c r="C314"/>
+      <c r="D314" s="4"/>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B315" s="2"/>
+      <c r="C315"/>
+      <c r="D315" s="4"/>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B316" s="2"/>
+      <c r="C316"/>
+      <c r="D316" s="4"/>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B317" s="2"/>
+      <c r="C317"/>
+      <c r="D317" s="4"/>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B318" s="2"/>
+      <c r="C318"/>
+      <c r="D318" s="4"/>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B319" s="2"/>
+      <c r="C319"/>
+      <c r="D319" s="4"/>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B320" s="2"/>
+      <c r="C320"/>
+      <c r="D320" s="4"/>
+    </row>
+    <row r="321" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B321" s="2"/>
+      <c r="C321"/>
+      <c r="D321" s="4"/>
+    </row>
+    <row r="322" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B322" s="2"/>
+      <c r="C322"/>
+      <c r="D322" s="4"/>
+    </row>
+    <row r="323" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B323" s="2"/>
+      <c r="C323"/>
+      <c r="D323" s="4"/>
+    </row>
+    <row r="324" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B324" s="2"/>
+      <c r="C324"/>
+      <c r="D324" s="4"/>
+    </row>
+    <row r="325" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B325" s="2"/>
+      <c r="C325"/>
+      <c r="D325" s="4"/>
+    </row>
+    <row r="326" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B326" s="2"/>
+      <c r="C326"/>
+      <c r="D326" s="4"/>
+    </row>
+    <row r="327" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B327" s="2"/>
+      <c r="C327"/>
+      <c r="D327" s="4"/>
+    </row>
+    <row r="328" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B328" s="2"/>
+      <c r="C328"/>
+      <c r="D328" s="4"/>
+    </row>
+    <row r="329" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B329" s="2"/>
+      <c r="C329"/>
+      <c r="D329" s="4"/>
+    </row>
+    <row r="330" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B330" s="2"/>
+      <c r="C330"/>
+      <c r="D330" s="4"/>
+    </row>
+    <row r="331" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B331" s="2"/>
+      <c r="C331"/>
+      <c r="D331" s="4"/>
+    </row>
+    <row r="332" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B332" s="2"/>
+      <c r="C332" s="2"/>
+      <c r="D332" s="2"/>
+      <c r="E332" s="2"/>
+    </row>
+    <row r="333" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B333" s="2"/>
+      <c r="C333" s="2"/>
+      <c r="D333" s="2"/>
+      <c r="E333" s="2"/>
+    </row>
+    <row r="334" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B334" s="2"/>
+      <c r="C334" s="2"/>
+      <c r="D334" s="2"/>
+      <c r="E334" s="2"/>
+    </row>
+    <row r="335" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B335" s="2"/>
+      <c r="C335" s="2"/>
+      <c r="D335" s="2"/>
+      <c r="E335" s="2"/>
+    </row>
+    <row r="336" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B336" s="2"/>
+      <c r="C336" s="2"/>
+      <c r="D336" s="2"/>
+      <c r="E336" s="2"/>
+    </row>
+    <row r="337" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+      <c r="D337" s="2"/>
+      <c r="E337" s="2"/>
+    </row>
+    <row r="338" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B338" s="2"/>
+      <c r="C338" s="2"/>
+      <c r="D338" s="2"/>
+      <c r="E338" s="2"/>
+    </row>
+    <row r="339" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B339" s="2"/>
+      <c r="C339" s="2"/>
+      <c r="D339" s="2"/>
+      <c r="E339" s="2"/>
+    </row>
+    <row r="340" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B340" s="2"/>
+      <c r="C340" s="2"/>
+      <c r="D340" s="2"/>
+      <c r="E340" s="2"/>
+    </row>
+    <row r="341" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B341" s="2"/>
+      <c r="C341" s="2"/>
+      <c r="D341" s="2"/>
+      <c r="E341" s="2"/>
+    </row>
+    <row r="342" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B342" s="2"/>
+      <c r="C342" s="2"/>
+      <c r="D342" s="2"/>
+      <c r="E342" s="2"/>
+    </row>
+    <row r="343" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B343" s="2"/>
+      <c r="C343" s="2"/>
+      <c r="D343" s="2"/>
+      <c r="E343" s="2"/>
+    </row>
+    <row r="344" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B344" s="2"/>
+      <c r="C344" s="2"/>
+      <c r="D344" s="2"/>
+      <c r="E344" s="2"/>
+    </row>
+    <row r="345" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B345" s="2"/>
+      <c r="C345" s="2"/>
+      <c r="D345" s="2"/>
+      <c r="E345" s="2"/>
+    </row>
+    <row r="346" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B346" s="2"/>
+      <c r="C346" s="2"/>
+      <c r="D346" s="2"/>
+      <c r="E346" s="2"/>
+    </row>
+    <row r="347" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B347" s="2"/>
+      <c r="C347" s="2"/>
+      <c r="D347" s="2"/>
+      <c r="E347" s="2"/>
+    </row>
+    <row r="348" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B348" s="2"/>
+      <c r="C348" s="2"/>
+      <c r="D348" s="2"/>
+      <c r="E348" s="2"/>
+    </row>
+    <row r="349" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B349" s="2"/>
+      <c r="C349" s="2"/>
+      <c r="D349" s="2"/>
+      <c r="E349" s="2"/>
+    </row>
+    <row r="350" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B350" s="2"/>
+      <c r="C350" s="2"/>
+      <c r="D350" s="2"/>
+      <c r="E350" s="2"/>
+    </row>
+    <row r="351" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B351" s="2"/>
+      <c r="C351" s="2"/>
+      <c r="D351" s="2"/>
+      <c r="E351" s="2"/>
+    </row>
+    <row r="352" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B352" s="2"/>
+      <c r="C352" s="2"/>
+      <c r="D352" s="2"/>
+      <c r="E352" s="2"/>
+    </row>
+    <row r="353" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B353" s="2"/>
+      <c r="C353" s="2"/>
+      <c r="D353" s="2"/>
+      <c r="E353" s="2"/>
+    </row>
+    <row r="354" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B354" s="2"/>
+      <c r="C354" s="2"/>
+      <c r="D354" s="2"/>
+      <c r="E354" s="2"/>
+    </row>
+    <row r="355" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B355" s="2"/>
+      <c r="C355" s="2"/>
+      <c r="D355" s="2"/>
+      <c r="E355" s="2"/>
+    </row>
+    <row r="356" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B356" s="2"/>
+      <c r="C356" s="2"/>
+      <c r="D356" s="2"/>
+      <c r="E356" s="2"/>
+    </row>
+    <row r="357" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B357" s="2"/>
+      <c r="C357" s="2"/>
+      <c r="D357" s="2"/>
+      <c r="E357" s="2"/>
+    </row>
+    <row r="358" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B358" s="2"/>
+      <c r="C358" s="2"/>
+      <c r="D358" s="2"/>
+      <c r="E358" s="2"/>
+    </row>
+    <row r="359" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B359" s="2"/>
+      <c r="C359" s="2"/>
+      <c r="D359" s="2"/>
+      <c r="E359" s="2"/>
+    </row>
+    <row r="360" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B360" s="2"/>
+      <c r="C360" s="2"/>
+      <c r="D360" s="2"/>
+      <c r="E360" s="2"/>
+    </row>
+    <row r="361" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B361" s="2"/>
+      <c r="C361" s="2"/>
+      <c r="D361" s="2"/>
+      <c r="E361" s="2"/>
+    </row>
+    <row r="362" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B362" s="2"/>
+      <c r="C362" s="2"/>
+      <c r="D362" s="2"/>
+      <c r="E362" s="2"/>
+    </row>
+    <row r="363" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B363" s="2"/>
+      <c r="C363" s="2"/>
+      <c r="D363" s="2"/>
+      <c r="E363" s="2"/>
+    </row>
+    <row r="364" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B364" s="2"/>
+      <c r="C364" s="2"/>
+      <c r="D364" s="2"/>
+      <c r="E364" s="2"/>
+    </row>
+    <row r="365" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B365" s="2"/>
+      <c r="C365" s="2"/>
+      <c r="D365" s="2"/>
+      <c r="E365" s="2"/>
+    </row>
+    <row r="366" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B366" s="2"/>
+      <c r="C366" s="2"/>
+      <c r="D366" s="2"/>
+      <c r="E366" s="2"/>
+    </row>
+    <row r="367" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B367" s="2"/>
+      <c r="C367" s="2"/>
+      <c r="D367" s="2"/>
+      <c r="E367" s="2"/>
+    </row>
+    <row r="368" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B368" s="2"/>
+      <c r="C368" s="2"/>
+      <c r="D368" s="2"/>
+      <c r="E368" s="2"/>
+    </row>
+    <row r="369" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B369" s="2"/>
+      <c r="C369" s="2"/>
+      <c r="D369" s="2"/>
+      <c r="E369" s="2"/>
+    </row>
+    <row r="370" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B370" s="2"/>
+      <c r="C370" s="2"/>
+      <c r="D370" s="2"/>
+      <c r="E370" s="2"/>
+    </row>
+    <row r="371" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B371" s="2"/>
+      <c r="C371" s="2"/>
+      <c r="D371" s="2"/>
+      <c r="E371" s="2"/>
+    </row>
+    <row r="372" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B372" s="2"/>
+      <c r="C372" s="2"/>
+      <c r="D372" s="2"/>
+      <c r="E372" s="2"/>
+    </row>
+    <row r="373" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B373" s="2"/>
+      <c r="C373" s="2"/>
+      <c r="D373" s="2"/>
+      <c r="E373" s="2"/>
+    </row>
+    <row r="374" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B374" s="2"/>
+      <c r="C374" s="2"/>
+      <c r="D374" s="2"/>
+      <c r="E374" s="2"/>
+    </row>
+    <row r="375" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B375" s="2"/>
+      <c r="C375" s="2"/>
+      <c r="D375" s="2"/>
+      <c r="E375" s="2"/>
+    </row>
+    <row r="376" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B376" s="2"/>
+      <c r="C376" s="2"/>
+      <c r="D376" s="2"/>
+      <c r="E376" s="2"/>
+    </row>
+    <row r="377" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B377" s="2"/>
+      <c r="C377" s="2"/>
+      <c r="D377" s="2"/>
+      <c r="E377" s="2"/>
+    </row>
+    <row r="378" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B378" s="2"/>
+      <c r="C378" s="2"/>
+      <c r="D378" s="2"/>
+      <c r="E378" s="2"/>
+    </row>
+    <row r="379" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B379" s="2"/>
+      <c r="C379" s="2"/>
+      <c r="D379" s="2"/>
+      <c r="E379" s="2"/>
+    </row>
+    <row r="380" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B380" s="2"/>
+      <c r="C380" s="2"/>
+      <c r="D380" s="2"/>
+      <c r="E380" s="2"/>
+    </row>
+    <row r="381" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B381" s="2"/>
+      <c r="C381" s="2"/>
+      <c r="D381" s="2"/>
+      <c r="E381" s="2"/>
+    </row>
+    <row r="382" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B382" s="2"/>
+      <c r="C382" s="2"/>
+      <c r="D382" s="2"/>
+      <c r="E382" s="2"/>
+    </row>
+    <row r="383" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B383" s="2"/>
+      <c r="C383" s="2"/>
+      <c r="D383" s="2"/>
+      <c r="E383" s="2"/>
+    </row>
+    <row r="384" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B384" s="2"/>
+      <c r="C384" s="2"/>
+      <c r="D384" s="2"/>
+      <c r="E384" s="2"/>
+    </row>
+    <row r="385" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B385" s="2"/>
+      <c r="C385" s="2"/>
+      <c r="D385" s="2"/>
+      <c r="E385" s="2"/>
+    </row>
+    <row r="386" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B386" s="2"/>
+      <c r="C386" s="2"/>
+      <c r="D386" s="2"/>
+      <c r="E386" s="2"/>
+    </row>
+    <row r="387" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B387" s="2"/>
+      <c r="C387" s="2"/>
+      <c r="D387" s="2"/>
+      <c r="E387" s="2"/>
+    </row>
+    <row r="388" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B388" s="2"/>
+      <c r="C388" s="2"/>
+      <c r="D388" s="2"/>
+      <c r="E388" s="2"/>
+    </row>
+    <row r="389" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B389" s="2"/>
+      <c r="C389" s="2"/>
+      <c r="D389" s="2"/>
+      <c r="E389" s="2"/>
+    </row>
+    <row r="390" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B390" s="2"/>
+      <c r="C390" s="2"/>
+      <c r="D390" s="2"/>
+      <c r="E390" s="2"/>
+    </row>
+    <row r="391" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B391" s="2"/>
+      <c r="C391" s="2"/>
+      <c r="D391" s="2"/>
+      <c r="E391" s="2"/>
+    </row>
+    <row r="392" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B392" s="2"/>
+      <c r="C392" s="2"/>
+      <c r="D392" s="2"/>
+      <c r="E392" s="2"/>
+    </row>
+    <row r="393" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B393" s="2"/>
+      <c r="C393" s="2"/>
+      <c r="D393" s="2"/>
+      <c r="E393" s="2"/>
+    </row>
+    <row r="394" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B394" s="2"/>
+      <c r="C394" s="2"/>
+      <c r="D394" s="2"/>
+      <c r="E394" s="2"/>
+    </row>
+    <row r="395" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B395" s="2"/>
+      <c r="C395" s="2"/>
+      <c r="D395" s="2"/>
+      <c r="E395" s="2"/>
+    </row>
+    <row r="396" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B396" s="2"/>
+      <c r="C396" s="2"/>
+      <c r="D396" s="2"/>
+      <c r="E396" s="2"/>
+    </row>
+    <row r="397" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B397" s="2"/>
+      <c r="C397" s="2"/>
+      <c r="D397" s="2"/>
+      <c r="E397" s="2"/>
+    </row>
+    <row r="398" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B398" s="2"/>
+      <c r="C398" s="2"/>
+      <c r="D398" s="2"/>
+      <c r="E398" s="2"/>
+    </row>
+    <row r="399" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B399" s="2"/>
+      <c r="C399" s="2"/>
+      <c r="D399" s="2"/>
+      <c r="E399" s="2"/>
+    </row>
+    <row r="400" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B400" s="2"/>
+      <c r="C400" s="2"/>
+      <c r="D400" s="2"/>
+      <c r="E400" s="2"/>
+    </row>
+    <row r="401" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B401" s="2"/>
+      <c r="C401" s="2"/>
+      <c r="D401" s="2"/>
+      <c r="E401" s="2"/>
+    </row>
+    <row r="402" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B402" s="2"/>
+      <c r="C402" s="2"/>
+      <c r="D402" s="2"/>
+      <c r="E402" s="2"/>
+    </row>
+    <row r="403" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B403" s="2"/>
+      <c r="C403" s="2"/>
+      <c r="D403" s="2"/>
+      <c r="E403" s="2"/>
+    </row>
+    <row r="404" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B404" s="2"/>
+      <c r="C404" s="2"/>
+      <c r="D404" s="2"/>
+      <c r="E404" s="2"/>
+    </row>
+    <row r="405" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B405" s="2"/>
+      <c r="C405" s="2"/>
+      <c r="D405" s="2"/>
+      <c r="E405" s="2"/>
+    </row>
+    <row r="406" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B406" s="2"/>
+      <c r="C406" s="2"/>
+      <c r="D406" s="2"/>
+      <c r="E406" s="2"/>
+    </row>
+    <row r="407" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B407" s="2"/>
+      <c r="C407" s="2"/>
+      <c r="D407" s="2"/>
+      <c r="E407" s="2"/>
+    </row>
+    <row r="408" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B408" s="2"/>
+      <c r="C408" s="2"/>
+      <c r="D408" s="2"/>
+      <c r="E408" s="2"/>
+    </row>
+    <row r="409" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B409" s="2"/>
+      <c r="C409" s="2"/>
+      <c r="D409" s="2"/>
+      <c r="E409" s="2"/>
+    </row>
+    <row r="410" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B410" s="2"/>
+      <c r="C410" s="2"/>
+      <c r="D410" s="2"/>
+      <c r="E410" s="2"/>
+    </row>
+    <row r="411" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B411" s="2"/>
+      <c r="C411" s="2"/>
+      <c r="D411" s="2"/>
+      <c r="E411" s="2"/>
+    </row>
+    <row r="412" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B412" s="2"/>
+      <c r="C412" s="2"/>
+      <c r="D412" s="2"/>
+      <c r="E412" s="2"/>
+    </row>
+    <row r="413" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B413" s="2"/>
+      <c r="C413" s="2"/>
+      <c r="D413" s="2"/>
+      <c r="E413" s="2"/>
+    </row>
+    <row r="414" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B414" s="2"/>
+      <c r="C414" s="2"/>
+      <c r="D414" s="2"/>
+      <c r="E414" s="2"/>
+    </row>
+    <row r="415" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B415" s="2"/>
+      <c r="C415" s="2"/>
+      <c r="D415" s="2"/>
+      <c r="E415" s="2"/>
+    </row>
+    <row r="416" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B416" s="2"/>
+      <c r="C416" s="2"/>
+      <c r="D416" s="2"/>
+      <c r="E416" s="2"/>
+    </row>
+    <row r="417" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B417" s="2"/>
+      <c r="C417" s="2"/>
+      <c r="D417" s="2"/>
+      <c r="E417" s="2"/>
+    </row>
+    <row r="418" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B418" s="2"/>
+      <c r="C418" s="2"/>
+      <c r="D418" s="2"/>
+      <c r="E418" s="2"/>
+    </row>
+    <row r="419" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B419" s="2"/>
+      <c r="C419" s="2"/>
+      <c r="D419" s="2"/>
+      <c r="E419" s="2"/>
+    </row>
+    <row r="420" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B420" s="2"/>
+      <c r="C420" s="2"/>
+      <c r="D420" s="2"/>
+      <c r="E420" s="2"/>
+    </row>
+    <row r="421" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B421" s="2"/>
+      <c r="C421" s="2"/>
+      <c r="D421" s="2"/>
+      <c r="E421" s="2"/>
+    </row>
+    <row r="422" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B422" s="2"/>
+      <c r="C422" s="2"/>
+      <c r="D422" s="2"/>
+      <c r="E422" s="2"/>
+    </row>
+    <row r="423" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B423" s="2"/>
+      <c r="C423" s="2"/>
+      <c r="D423" s="2"/>
+      <c r="E423" s="2"/>
+    </row>
+    <row r="424" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B424" s="2"/>
+      <c r="C424" s="2"/>
+      <c r="D424" s="2"/>
+      <c r="E424" s="2"/>
+    </row>
+    <row r="425" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B425" s="2"/>
+      <c r="C425" s="2"/>
+      <c r="D425" s="2"/>
+      <c r="E425" s="2"/>
+    </row>
+    <row r="426" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B426" s="2"/>
+      <c r="C426" s="2"/>
+      <c r="D426" s="2"/>
+      <c r="E426" s="2"/>
+    </row>
+    <row r="427" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B427" s="2"/>
+      <c r="C427" s="2"/>
+      <c r="D427" s="2"/>
+      <c r="E427" s="2"/>
+    </row>
+    <row r="428" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B428" s="2"/>
+      <c r="C428" s="2"/>
+      <c r="D428" s="2"/>
+      <c r="E428" s="2"/>
+    </row>
+    <row r="429" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B429" s="2"/>
+      <c r="C429" s="2"/>
+      <c r="D429" s="2"/>
+      <c r="E429" s="2"/>
+    </row>
+    <row r="430" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B430" s="2"/>
+      <c r="C430" s="2"/>
+      <c r="D430" s="2"/>
+      <c r="E430" s="2"/>
+    </row>
+    <row r="431" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B431" s="2"/>
+      <c r="C431" s="2"/>
+      <c r="D431" s="2"/>
+      <c r="E431" s="2"/>
+    </row>
+    <row r="432" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B432" s="2"/>
+      <c r="C432" s="2"/>
+      <c r="D432" s="2"/>
+      <c r="E432" s="2"/>
+    </row>
+    <row r="433" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B433" s="2"/>
+      <c r="C433" s="2"/>
+      <c r="D433" s="2"/>
+      <c r="E433" s="2"/>
+    </row>
+    <row r="434" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B434" s="2"/>
+      <c r="C434" s="2"/>
+      <c r="D434" s="2"/>
+      <c r="E434" s="2"/>
+    </row>
+    <row r="435" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B435" s="2"/>
+      <c r="C435" s="2"/>
+      <c r="D435" s="2"/>
+      <c r="E435" s="2"/>
+    </row>
+    <row r="436" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B436" s="2"/>
+      <c r="C436" s="2"/>
+      <c r="D436" s="2"/>
+      <c r="E436" s="2"/>
+    </row>
+    <row r="437" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B437" s="2"/>
+      <c r="C437" s="2"/>
+      <c r="D437" s="2"/>
+      <c r="E437" s="2"/>
+    </row>
+    <row r="438" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B438" s="2"/>
+      <c r="C438" s="2"/>
+      <c r="D438" s="2"/>
+      <c r="E438" s="2"/>
+    </row>
+    <row r="439" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B439" s="2"/>
+      <c r="C439" s="2"/>
+      <c r="D439" s="2"/>
+      <c r="E439" s="2"/>
+    </row>
+    <row r="440" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B440" s="2"/>
+      <c r="C440" s="2"/>
+      <c r="D440" s="2"/>
+      <c r="E440" s="2"/>
+    </row>
+    <row r="441" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B441" s="2"/>
+      <c r="C441" s="2"/>
+      <c r="D441" s="2"/>
+      <c r="E441" s="2"/>
+    </row>
+    <row r="442" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B442" s="2"/>
+      <c r="C442" s="2"/>
+      <c r="D442" s="2"/>
+      <c r="E442" s="2"/>
+    </row>
+    <row r="443" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B443" s="2"/>
+      <c r="C443" s="2"/>
+      <c r="D443" s="2"/>
+      <c r="E443" s="2"/>
+    </row>
+    <row r="444" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B444" s="2"/>
+      <c r="C444" s="2"/>
+      <c r="D444" s="2"/>
+      <c r="E444" s="2"/>
+    </row>
+    <row r="445" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B445" s="2"/>
+      <c r="C445" s="2"/>
+      <c r="D445" s="2"/>
+      <c r="E445" s="2"/>
+    </row>
+    <row r="446" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B446" s="2"/>
+      <c r="C446" s="2"/>
+      <c r="D446" s="2"/>
+      <c r="E446" s="2"/>
+    </row>
+    <row r="447" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B447" s="2"/>
+      <c r="C447" s="2"/>
+      <c r="D447" s="2"/>
+      <c r="E447" s="2"/>
+    </row>
+    <row r="448" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B448" s="2"/>
+      <c r="C448" s="2"/>
+      <c r="D448" s="2"/>
+      <c r="E448" s="2"/>
+    </row>
+    <row r="449" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B449" s="2"/>
+      <c r="C449" s="2"/>
+      <c r="D449" s="2"/>
+      <c r="E449" s="2"/>
+    </row>
+    <row r="450" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B450" s="2"/>
+      <c r="C450" s="2"/>
+      <c r="D450" s="2"/>
+      <c r="E450" s="2"/>
+    </row>
+    <row r="451" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B451" s="2"/>
+      <c r="C451" s="2"/>
+      <c r="D451" s="2"/>
+      <c r="E451" s="2"/>
+    </row>
+    <row r="452" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B452" s="2"/>
+      <c r="C452" s="2"/>
+      <c r="D452" s="2"/>
+      <c r="E452" s="2"/>
+    </row>
+    <row r="453" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B453" s="2"/>
+      <c r="C453" s="2"/>
+      <c r="D453" s="2"/>
+      <c r="E453" s="2"/>
+    </row>
+    <row r="454" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B454" s="2"/>
+      <c r="C454" s="2"/>
+      <c r="D454" s="2"/>
+      <c r="E454" s="2"/>
+    </row>
+    <row r="455" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B455" s="2"/>
+      <c r="C455" s="2"/>
+      <c r="D455" s="2"/>
+      <c r="E455" s="2"/>
+    </row>
+    <row r="456" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B456" s="2"/>
+      <c r="C456" s="2"/>
+      <c r="D456" s="2"/>
+      <c r="E456" s="2"/>
+    </row>
+    <row r="457" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B457" s="2"/>
+      <c r="C457" s="2"/>
+      <c r="D457" s="2"/>
+      <c r="E457" s="2"/>
+    </row>
+    <row r="458" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B458" s="2"/>
+      <c r="C458" s="2"/>
+      <c r="D458" s="2"/>
+      <c r="E458" s="2"/>
+    </row>
+    <row r="459" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B459" s="2"/>
+      <c r="C459" s="2"/>
+      <c r="D459" s="2"/>
+      <c r="E459" s="2"/>
+    </row>
+    <row r="460" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B460" s="2"/>
+      <c r="C460" s="2"/>
+      <c r="D460" s="2"/>
+      <c r="E460" s="2"/>
+    </row>
+    <row r="461" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B461" s="2"/>
+      <c r="C461" s="2"/>
+      <c r="D461" s="2"/>
+      <c r="E461" s="2"/>
+    </row>
+    <row r="462" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B462" s="2"/>
+      <c r="C462" s="2"/>
+      <c r="D462" s="2"/>
+      <c r="E462" s="2"/>
+    </row>
+    <row r="463" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B463" s="2"/>
+      <c r="C463" s="2"/>
+      <c r="D463" s="2"/>
+      <c r="E463" s="2"/>
+    </row>
+    <row r="464" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B464" s="2"/>
+      <c r="C464" s="2"/>
+      <c r="D464" s="2"/>
+      <c r="E464" s="2"/>
+    </row>
+    <row r="465" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B465" s="2"/>
+      <c r="C465" s="2"/>
+      <c r="D465" s="2"/>
+      <c r="E465" s="2"/>
+    </row>
+    <row r="466" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B466" s="2"/>
+      <c r="C466" s="2"/>
+      <c r="D466" s="2"/>
+      <c r="E466" s="2"/>
+    </row>
+    <row r="467" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B467" s="2"/>
+      <c r="C467" s="2"/>
+      <c r="D467" s="2"/>
+      <c r="E467" s="2"/>
+    </row>
+    <row r="468" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B468" s="2"/>
+      <c r="C468" s="2"/>
+      <c r="D468" s="2"/>
+      <c r="E468" s="2"/>
+    </row>
+    <row r="469" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B469" s="2"/>
+      <c r="C469" s="2"/>
+      <c r="D469" s="2"/>
+      <c r="E469" s="2"/>
+    </row>
+    <row r="470" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B470" s="2"/>
+      <c r="C470" s="2"/>
+      <c r="D470" s="2"/>
+      <c r="E470" s="2"/>
+    </row>
+    <row r="471" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B471" s="2"/>
+      <c r="C471" s="2"/>
+      <c r="D471" s="2"/>
+      <c r="E471" s="2"/>
+    </row>
+    <row r="472" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B472" s="2"/>
+      <c r="C472" s="2"/>
+      <c r="D472" s="2"/>
+      <c r="E472" s="2"/>
+    </row>
+    <row r="473" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B473" s="2"/>
+      <c r="C473" s="2"/>
+      <c r="D473" s="2"/>
+      <c r="E473" s="2"/>
+    </row>
+    <row r="474" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B474" s="2"/>
+      <c r="C474" s="2"/>
+      <c r="D474" s="2"/>
+      <c r="E474" s="2"/>
+    </row>
+    <row r="475" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B475" s="2"/>
+      <c r="C475" s="2"/>
+      <c r="D475" s="2"/>
+      <c r="E475" s="2"/>
+    </row>
+    <row r="476" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B476" s="2"/>
+      <c r="C476" s="2"/>
+      <c r="D476" s="2"/>
+      <c r="E476" s="2"/>
+    </row>
+    <row r="477" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B477" s="2"/>
+      <c r="C477" s="2"/>
+      <c r="D477" s="2"/>
+      <c r="E477" s="2"/>
+    </row>
+    <row r="478" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B478" s="2"/>
+      <c r="C478" s="2"/>
+      <c r="D478" s="2"/>
+      <c r="E478" s="2"/>
+    </row>
+    <row r="479" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B479" s="2"/>
+      <c r="C479" s="2"/>
+      <c r="D479" s="2"/>
+      <c r="E479" s="2"/>
+    </row>
+    <row r="480" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B480" s="2"/>
+      <c r="C480" s="2"/>
+      <c r="D480" s="2"/>
+      <c r="E480" s="2"/>
+    </row>
+    <row r="481" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B481" s="2"/>
+      <c r="C481" s="2"/>
+      <c r="D481" s="2"/>
+      <c r="E481" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>

</xml_diff>